<commit_message>
feat: Nova versão do ROTEIRO roteiro_v3.png
</commit_message>
<xml_diff>
--- a/docs/roteiro_op.xlsx
+++ b/docs/roteiro_op.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\REPOSITORIOS\eureka_app_pyqt5_project-dev_v2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2A4D54-101D-483D-A471-33A318B17401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9587A501-B1E5-4312-9D97-0A6D6CC1CDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B165DDD0-5F89-4DC2-A807-872E8C7D4087}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="29">
   <si>
     <t>CORTE</t>
   </si>
@@ -126,6 +126,9 @@
   <si>
     <t>MONTAGEM
 MECÂNICA</t>
+  </si>
+  <si>
+    <t>Anotações:</t>
   </si>
 </sst>
 </file>
@@ -230,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -575,11 +578,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -612,9 +644,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -645,15 +674,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -687,23 +707,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -712,6 +723,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1230,10 +1271,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="E1:S15"/>
+  <dimension ref="E1:S20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,115 +1291,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
     </row>
     <row r="2" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="42">
         <v>1</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="23">
+      <c r="G2" s="43"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="42">
         <v>2</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="23">
+      <c r="J2" s="43"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="42">
         <v>3</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="23">
+      <c r="M2" s="43"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="42">
         <v>4</v>
       </c>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="25"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="44"/>
     </row>
     <row r="3" spans="5:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="34" t="s">
+      <c r="I3" s="32"/>
+      <c r="J3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="34" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="36"/>
-      <c r="P3" s="34" t="s">
+      <c r="O3" s="32"/>
+      <c r="P3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="35" t="s">
+      <c r="Q3" s="31" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="15" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="12"/>
+      <c r="P4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="25" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="6"/>
@@ -1391,40 +1432,40 @@
       </c>
     </row>
     <row r="6" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="O6" s="17"/>
-      <c r="P6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q6" s="19" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="16"/>
+      <c r="M6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="16"/>
+      <c r="P6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="25" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="6"/>
@@ -1457,40 +1498,40 @@
       </c>
     </row>
     <row r="8" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="17"/>
-      <c r="M8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" s="17"/>
-      <c r="P8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" s="19" t="s">
+      <c r="F8" s="16"/>
+      <c r="G8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="16"/>
+      <c r="M8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="16"/>
+      <c r="P8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="25" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="6"/>
@@ -1523,41 +1564,41 @@
       </c>
     </row>
     <row r="10" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="20"/>
-      <c r="M10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="N10" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="S10" s="45"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="19"/>
+      <c r="J10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="19"/>
+      <c r="M10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" s="38"/>
     </row>
     <row r="11" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="6"/>
@@ -1590,40 +1631,40 @@
       </c>
     </row>
     <row r="12" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="17"/>
-      <c r="M12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" s="17"/>
-      <c r="P12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q12" s="19" t="s">
+      <c r="F12" s="16"/>
+      <c r="G12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="16"/>
+      <c r="M12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="16"/>
+      <c r="P12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="9"/>
@@ -1656,47 +1697,111 @@
       </c>
     </row>
     <row r="14" spans="5:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E14" s="38"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
     </row>
     <row r="15" spans="5:19" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="43"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="39" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="39"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="42" t="s">
+      <c r="I15" s="37"/>
+      <c r="J15" s="40" t="s">
         <v>26</v>
       </c>
       <c r="K15" s="39"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="42" t="s">
+      <c r="L15" s="37"/>
+      <c r="M15" s="40" t="s">
         <v>27</v>
       </c>
       <c r="N15" s="39"/>
-      <c r="O15" s="44"/>
+      <c r="O15" s="37"/>
       <c r="P15" s="39" t="s">
         <v>25</v>
       </c>
       <c r="Q15" s="39"/>
     </row>
+    <row r="16" spans="5:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E17" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+    </row>
+    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E18" s="45"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46"/>
+    </row>
+    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E19" s="45"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="46"/>
+      <c r="Q19" s="46"/>
+    </row>
+    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E20" s="47"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="E17:Q20"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="M15:N15"/>

</xml_diff>

<commit_message>
feat: Adicionado função para gerar o código de barras conforme o número da da Ordem de Produção. Módulo de PCP
</commit_message>
<xml_diff>
--- a/docs/roteiro_op.xlsx
+++ b/docs/roteiro_op.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\REPOSITORIOS\eureka_app_pyqt5_project-dev_v2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9587A501-B1E5-4312-9D97-0A6D6CC1CDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B2DFAA-F2F4-4409-BBD4-31D1874C0376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B165DDD0-5F89-4DC2-A807-872E8C7D4087}"/>
   </bookViews>
@@ -135,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +212,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -233,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -578,40 +584,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -741,16 +718,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1274,7 +1242,7 @@
   <dimension ref="E1:S20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,76 +1709,76 @@
       <c r="E17" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E18" s="45"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
     </row>
     <row r="19" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E19" s="45"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="Q19" s="46"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E20" s="47"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E1:Q1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
     <mergeCell ref="E17:Q20"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="E1:Q1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="47" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
:sparkles: feat: Adicionado nova funcionalidade. Seleção múltipla de linhas da tabela para Imprimir OP. Módulo PCP
</commit_message>
<xml_diff>
--- a/docs/roteiro_op.xlsx
+++ b/docs/roteiro_op.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\REPOSITORIOS\eureka_app_pyqt5_project-dev_v2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B2DFAA-F2F4-4409-BBD4-31D1874C0376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F4B024-31E4-41E5-A10F-5E6723F76FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B165DDD0-5F89-4DC2-A807-872E8C7D4087}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B165DDD0-5F89-4DC2-A807-872E8C7D4087}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="29">
   <si>
     <t>CORTE</t>
   </si>
@@ -700,26 +701,26 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1241,7 +1242,7 @@
   </sheetPr>
   <dimension ref="E1:S20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
@@ -1259,46 +1260,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
     </row>
     <row r="2" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="42">
+      <c r="F2" s="40">
         <v>1</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="42">
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="40">
         <v>2</v>
       </c>
-      <c r="J2" s="43"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="42">
+      <c r="J2" s="41"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="40">
         <v>3</v>
       </c>
-      <c r="M2" s="43"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="42">
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="40">
         <v>4</v>
       </c>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="44"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="42"/>
     </row>
     <row r="3" spans="5:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="23" t="s">
@@ -1684,97 +1685,648 @@
         <v>24</v>
       </c>
       <c r="F15" s="36"/>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="39"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="37"/>
-      <c r="J15" s="40" t="s">
+      <c r="J15" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="39"/>
+      <c r="K15" s="44"/>
       <c r="L15" s="37"/>
-      <c r="M15" s="40" t="s">
+      <c r="M15" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="N15" s="39"/>
+      <c r="N15" s="44"/>
       <c r="O15" s="37"/>
-      <c r="P15" s="39" t="s">
+      <c r="P15" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="Q15" s="39"/>
+      <c r="Q15" s="44"/>
     </row>
     <row r="16" spans="5:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
     </row>
     <row r="19" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E17:Q20"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="P15:Q15"/>
     <mergeCell ref="E1:Q1"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="O2:Q2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" scale="47" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F860DE-FE8A-4E8A-B83E-33BB9E27F137}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="E1:S20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" customWidth="1"/>
+    <col min="10" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" customWidth="1"/>
+    <col min="16" max="17" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+    </row>
+    <row r="2" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="40">
+        <v>1</v>
+      </c>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="40">
+        <v>2</v>
+      </c>
+      <c r="J2" s="41"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="40">
+        <v>3</v>
+      </c>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="40">
+        <v>4</v>
+      </c>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="42"/>
+    </row>
+    <row r="3" spans="5:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="32"/>
+      <c r="M3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="32"/>
+      <c r="P3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="12"/>
+      <c r="P4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="16"/>
+      <c r="M6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="16"/>
+      <c r="P6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="6"/>
+      <c r="P7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="16"/>
+      <c r="M8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="16"/>
+      <c r="P8" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="19"/>
+      <c r="J10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="19"/>
+      <c r="M10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" s="38"/>
+    </row>
+    <row r="11" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="6"/>
+      <c r="M11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="6"/>
+      <c r="P11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="16"/>
+      <c r="M12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="16"/>
+      <c r="P12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" s="9"/>
+      <c r="P13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="5:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="34"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+    </row>
+    <row r="15" spans="5:19" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="44"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="44"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="44"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q15" s="44"/>
+    </row>
+    <row r="16" spans="5:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E17" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+    </row>
+    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
+    </row>
+    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+    </row>
+    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
     <mergeCell ref="E17:Q20"/>
+    <mergeCell ref="E1:Q1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="M15:N15"/>

</xml_diff>

<commit_message>
:recycle: refactor: Atualizado requirements.txt e template dos roteiros
</commit_message>
<xml_diff>
--- a/docs/roteiro_op.xlsx
+++ b/docs/roteiro_op.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\REPOSITORIOS\eureka_app_pyqt5_project-dev_v2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F4B024-31E4-41E5-A10F-5E6723F76FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861159FF-2B1F-4DC0-9F21-08E6516391D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B165DDD0-5F89-4DC2-A807-872E8C7D4087}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
+    <sheet name="Planilha4" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="41">
   <si>
     <t>CORTE</t>
   </si>
@@ -130,13 +131,51 @@
   </si>
   <si>
     <t>Anotações:</t>
+  </si>
+  <si>
+    <t>SEQ.</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>HORA
+INÍCIO</t>
+  </si>
+  <si>
+    <t>HORA
+FIM</t>
+  </si>
+  <si>
+    <t>□ ESTOQUE</t>
+  </si>
+  <si>
+    <t>□ MONTAGEM MECÂNICA</t>
+  </si>
+  <si>
+    <t>□ USINAGEM</t>
+  </si>
+  <si>
+    <t>□ MONTAGEM        CALDEIRARIA</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>DATA INÍCIO</t>
+  </si>
+  <si>
+    <t>HORA INÍCIO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +258,15 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,8 +285,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -585,11 +637,232 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -701,16 +974,120 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -721,6 +1098,39 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1260,46 +1670,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
     </row>
     <row r="2" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="40">
+      <c r="F2" s="83">
         <v>1</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="40">
+      <c r="G2" s="84"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="83">
         <v>2</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="40">
+      <c r="J2" s="84"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="83">
         <v>3</v>
       </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="40">
+      <c r="M2" s="84"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="83">
         <v>4</v>
       </c>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="42"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="85"/>
     </row>
     <row r="3" spans="5:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="23" t="s">
@@ -1685,101 +2095,101 @@
         <v>24</v>
       </c>
       <c r="F15" s="36"/>
-      <c r="G15" s="44" t="s">
+      <c r="G15" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="44"/>
+      <c r="H15" s="80"/>
       <c r="I15" s="37"/>
-      <c r="J15" s="45" t="s">
+      <c r="J15" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="44"/>
+      <c r="K15" s="80"/>
       <c r="L15" s="37"/>
-      <c r="M15" s="45" t="s">
+      <c r="M15" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="N15" s="44"/>
+      <c r="N15" s="80"/>
       <c r="O15" s="37"/>
-      <c r="P15" s="44" t="s">
+      <c r="P15" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="Q15" s="44"/>
+      <c r="Q15" s="80"/>
     </row>
     <row r="16" spans="5:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="79"/>
+      <c r="P17" s="79"/>
+      <c r="Q17" s="79"/>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="43"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="79"/>
     </row>
     <row r="19" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="43"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="79"/>
+      <c r="O19" s="79"/>
+      <c r="P19" s="79"/>
+      <c r="Q19" s="79"/>
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="43"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="79"/>
+      <c r="O20" s="79"/>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E1:Q1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
     <mergeCell ref="E17:Q20"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="E1:Q1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="47" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1791,548 +2201,951 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="E1:S20"/>
+  <dimension ref="E1:O18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="S17" sqref="S17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="15" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="92" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+    </row>
+    <row r="2" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="86" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="86"/>
+      <c r="G2" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="89" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="89" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="88"/>
+    </row>
+    <row r="3" spans="5:15" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="78" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="5:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="5:15" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="5:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+    </row>
+    <row r="16" spans="5:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+    </row>
+    <row r="17" spans="5:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+    </row>
+    <row r="18" spans="5:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="E1:O1"/>
+    <mergeCell ref="E15:K18"/>
+    <mergeCell ref="E2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" scale="87" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D200ADD-DD11-4048-8462-F01F4E52F562}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="E1:Q20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.7109375" customWidth="1"/>
-    <col min="7" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" customWidth="1"/>
-    <col min="10" max="11" width="14.7109375" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" customWidth="1"/>
-    <col min="13" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" customWidth="1"/>
-    <col min="16" max="17" width="14.7109375" customWidth="1"/>
+    <col min="7" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" customWidth="1"/>
+    <col min="12" max="15" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E1" s="39" t="s">
+    <row r="1" spans="5:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-    </row>
-    <row r="2" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="22" t="s">
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+    </row>
+    <row r="2" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="40">
+      <c r="F2" s="89">
         <v>1</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="40">
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="89">
         <v>2</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="40">
-        <v>3</v>
-      </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="40">
-        <v>4</v>
-      </c>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="42"/>
-    </row>
-    <row r="3" spans="5:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="88"/>
+    </row>
+    <row r="3" spans="5:17" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="23" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="32"/>
-      <c r="M3" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="32"/>
-      <c r="P3" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="31" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="32"/>
+      <c r="L3" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="25" t="s">
+      <c r="F4" s="71"/>
+      <c r="G4" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="71"/>
+      <c r="L4" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="26" t="s">
+      <c r="F5" s="72"/>
+      <c r="G5" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="72"/>
+      <c r="L5" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="O6" s="16"/>
-      <c r="P6" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q6" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="25" t="s">
+      <c r="F6" s="73"/>
+      <c r="G6" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="73"/>
+      <c r="L6" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="27" t="s">
+      <c r="F7" s="72"/>
+      <c r="G7" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="72"/>
+      <c r="L7" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="N8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" s="16"/>
-      <c r="P8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="25" t="s">
+      <c r="F8" s="73"/>
+      <c r="G8" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="73"/>
+      <c r="L8" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="27" t="s">
+      <c r="F9" s="72"/>
+      <c r="G9" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="72"/>
+      <c r="L9" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="19"/>
-      <c r="M10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="N10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="O10" s="19"/>
-      <c r="P10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="S10" s="38"/>
-    </row>
-    <row r="11" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="25" t="s">
+      <c r="F10" s="73"/>
+      <c r="G10" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="73"/>
+      <c r="L10" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="38"/>
+    </row>
+    <row r="11" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q11" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="27" t="s">
+      <c r="F11" s="72"/>
+      <c r="G11" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="72"/>
+      <c r="L11" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" s="16"/>
-      <c r="P12" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q12" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="5:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="28" t="s">
+      <c r="F12" s="73"/>
+      <c r="G12" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="73"/>
+      <c r="L12" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="5:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="O13" s="9"/>
-      <c r="P13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q13" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="5:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="72"/>
+      <c r="G13" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="72"/>
+      <c r="L13" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="5:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E14" s="34"/>
       <c r="F14" s="3"/>
       <c r="G14" s="33"/>
       <c r="H14" s="33"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="33"/>
       <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="33"/>
       <c r="M14" s="33"/>
       <c r="N14" s="33"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
-    </row>
-    <row r="15" spans="5:19" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="35" t="s">
+      <c r="O14" s="33"/>
+    </row>
+    <row r="15" spans="5:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="44"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="K15" s="44"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="44"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q15" s="44"/>
-    </row>
-    <row r="16" spans="5:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E17" s="43" t="s">
+      <c r="F15" s="57"/>
+      <c r="G15" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="90"/>
+      <c r="I15" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="90"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="91" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="90"/>
+      <c r="N15" s="90" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" s="90"/>
+    </row>
+    <row r="16" spans="5:17" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E17" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
-    </row>
-    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="43"/>
-    </row>
-    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="43"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="43"/>
-    </row>
-    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="43"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="79"/>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="79"/>
+      <c r="O19" s="79"/>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="79"/>
+      <c r="O20" s="79"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="E17:Q20"/>
-    <mergeCell ref="E1:Q1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
+  <mergeCells count="8">
+    <mergeCell ref="E17:O20"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="E1:O1"/>
     <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="47" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="50" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>